<commit_message>
Added USART basic configuration
</commit_message>
<xml_diff>
--- a/Encoder Characteristics.xlsx
+++ b/Encoder Characteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pauld\Programming\NN54\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC58681-75FE-47B0-A7C4-B210413F807D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534E88C4-3762-4218-824F-9E4DE0855527}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encoder Error" sheetId="1" r:id="rId1"/>
@@ -313,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -346,6 +346,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -373,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,6 +422,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +491,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -784,7 +793,7 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -13494,7 +13503,7 @@
       <selection activeCell="I123" sqref="I123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
@@ -19266,11 +19275,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3BDFF7-A03C-4436-BDC7-9DE4C8404CC4}">
   <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
@@ -19300,8 +19309,8 @@
       <c r="H4">
         <v>14.9</v>
       </c>
-      <c r="I4">
-        <v>0</v>
+      <c r="I4" s="20">
+        <v>0.41399999999999998</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -19323,17 +19332,18 @@
         <v>21</v>
       </c>
       <c r="H6">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I6">
         <v>3</v>
       </c>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>22</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="20">
         <v>15</v>
       </c>
       <c r="I7">
@@ -19357,11 +19367,11 @@
       </c>
       <c r="H9">
         <f>SUM(H4:H8)</f>
-        <v>65.900000000000006</v>
+        <v>53.9</v>
       </c>
       <c r="I9">
         <f>SUM(I4:I8)</f>
-        <v>25</v>
+        <v>25.414000000000001</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -19370,11 +19380,11 @@
       </c>
       <c r="H11">
         <f>L5/H9</f>
-        <v>53.110773899848247</v>
+        <v>64.935064935064943</v>
       </c>
       <c r="I11">
         <f>L5/I9</f>
-        <v>140</v>
+        <v>137.71936727787832</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -19383,11 +19393,11 @@
       </c>
       <c r="H12">
         <f>H11/4</f>
-        <v>13.277693474962062</v>
+        <v>16.233766233766236</v>
       </c>
       <c r="I12">
         <f>I11/4</f>
-        <v>35</v>
+        <v>34.42984181946958</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -19481,6 +19491,7 @@
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19492,7 +19503,7 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="12.88671875" customWidth="1"/>
@@ -19775,11 +19786,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9794E4-8E8D-461D-9918-F078072C3809}">
   <dimension ref="A4:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="10.44140625" customWidth="1"/>
     <col min="13" max="13" width="12.109375" customWidth="1"/>
@@ -19835,7 +19846,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <f>A6+0.1</f>
+        <f t="shared" ref="E6:E17" si="0">A6+0.1</f>
         <v>0.1</v>
       </c>
       <c r="F6">
@@ -19855,19 +19866,19 @@
         <v>0.99959999999999993</v>
       </c>
       <c r="L6">
-        <f>F6-B6</f>
+        <f t="shared" ref="L6:L17" si="1">F6-B6</f>
         <v>1.7453283658983088E-3</v>
       </c>
       <c r="M6" s="15">
-        <f>G6-C6</f>
+        <f t="shared" ref="M6:M17" si="2">G6-C6</f>
         <v>-1.5230867123072755E-6</v>
       </c>
       <c r="O6">
-        <f>DEGREES(ATAN2(G6,F6))</f>
+        <f t="shared" ref="O6:O17" si="3">DEGREES(ATAN2(G6,F6))</f>
         <v>0.1</v>
       </c>
       <c r="P6">
-        <f>DEGREES(ATAN2(I6,F6))</f>
+        <f t="shared" ref="P6:P17" si="4">DEGREES(ATAN2(I6,F6))</f>
         <v>9.9979851761888963E-2</v>
       </c>
       <c r="Q6">
@@ -19888,7 +19899,7 @@
         <v>0.99619469809174555</v>
       </c>
       <c r="E7">
-        <f>A7+0.1</f>
+        <f t="shared" si="0"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="F7">
@@ -19900,31 +19911,31 @@
         <v>0.99604106541076953</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I17" si="0">ROUND(G7/0.0006,0)*0.0006</f>
+        <f t="shared" ref="I7:I17" si="5">ROUND(G7/0.0006,0)*0.0006</f>
         <v>0.99599999999999989</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J17" si="1">TRUNC(G7/0.0006,0)*0.0006</f>
+        <f t="shared" ref="J7:J17" si="6">TRUNC(G7/0.0006,0)*0.0006</f>
         <v>0.99599999999999989</v>
       </c>
       <c r="L7">
-        <f>F7-B7</f>
+        <f t="shared" si="1"/>
         <v>1.7385541187833475E-3</v>
       </c>
       <c r="M7" s="16">
-        <f>G7-C7</f>
+        <f t="shared" si="2"/>
         <v>-1.5363268097601246E-4</v>
       </c>
       <c r="O7">
-        <f>DEGREES(ATAN2(G7,F7))</f>
+        <f t="shared" si="3"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="P7">
-        <f>DEGREES(ATAN2(I7,F7))</f>
+        <f t="shared" si="4"/>
         <v>5.1002091656994137</v>
       </c>
       <c r="Q7">
-        <f t="shared" ref="Q7:Q17" si="2">DEGREES(ATAN2(J7,F7))</f>
+        <f t="shared" ref="Q7:Q17" si="7">DEGREES(ATAN2(J7,F7))</f>
         <v>5.1002091656994137</v>
       </c>
     </row>
@@ -19933,51 +19944,51 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B11" si="3">SIN(RADIANS(A8))</f>
+        <f t="shared" ref="B8:B11" si="8">SIN(RADIANS(A8))</f>
         <v>0.17364817766693033</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C11" si="4">COS(RADIANS(A8))</f>
+        <f t="shared" ref="C8:C11" si="9">COS(RADIANS(A8))</f>
         <v>0.98480775301220802</v>
       </c>
       <c r="E8">
-        <f>A8+0.1</f>
+        <f t="shared" si="0"/>
         <v>10.1</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F11" si="5">SIN(RADIANS(E8))</f>
+        <f t="shared" ref="F8:F11" si="10">SIN(RADIANS(E8))</f>
         <v>0.17536672609198711</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G11" si="6">COS(RADIANS(E8))</f>
+        <f t="shared" ref="G8:G11" si="11">COS(RADIANS(E8))</f>
         <v>0.98450317997443659</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.98459999999999992</v>
       </c>
       <c r="J8">
+        <f t="shared" si="6"/>
+        <v>0.98399999999999987</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="1"/>
-        <v>0.98399999999999987</v>
-      </c>
-      <c r="L8">
-        <f>F8-B8</f>
         <v>1.7185484250567817E-3</v>
       </c>
       <c r="M8">
-        <f>G8-C8</f>
+        <f t="shared" si="2"/>
         <v>-3.045730377714273E-4</v>
       </c>
       <c r="O8">
-        <f>DEGREES(ATAN2(G8,F8))</f>
+        <f t="shared" si="3"/>
         <v>10.100000000000001</v>
       </c>
       <c r="P8">
-        <f>DEGREES(ATAN2(I8,F8))</f>
+        <f t="shared" si="4"/>
         <v>10.099027267055572</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>10.105058344099122</v>
       </c>
     </row>
@@ -19986,51 +19997,51 @@
         <v>20</v>
       </c>
       <c r="B9">
+        <f t="shared" si="8"/>
+        <v>0.34202014332566871</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="9"/>
+        <v>0.93969262078590843</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>20.100000000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="10"/>
+        <v>0.34365969458561607</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="11"/>
+        <v>0.93909425209470909</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="6"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>1.6395512599473583E-3</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>-5.9836869119933578E-4</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="3"/>
-        <v>0.34202014332566871</v>
-      </c>
-      <c r="C9">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="4"/>
-        <v>0.93969262078590843</v>
-      </c>
-      <c r="E9">
-        <f>A9+0.1</f>
-        <v>20.100000000000001</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="5"/>
-        <v>0.34365969458561607</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="6"/>
-        <v>0.93909425209470909</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0.93899999999999995</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
-        <v>0.93899999999999995</v>
-      </c>
-      <c r="L9">
-        <f>F9-B9</f>
-        <v>1.6395512599473583E-3</v>
-      </c>
-      <c r="M9">
-        <f>G9-C9</f>
-        <v>-5.9836869119933578E-4</v>
-      </c>
-      <c r="O9">
-        <f>DEGREES(ATAN2(G9,F9))</f>
-        <v>20.100000000000001</v>
-      </c>
-      <c r="P9">
-        <f>DEGREES(ATAN2(I9,F9))</f>
         <v>20.101856011594094</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>20.101856011594094</v>
       </c>
     </row>
@@ -20039,51 +20050,51 @@
         <v>30</v>
       </c>
       <c r="B10">
+        <f t="shared" si="8"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="9"/>
+        <v>0.86602540378443871</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>30.1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="10"/>
+        <v>0.50151073715945738</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="11"/>
+        <v>0.8651514205697044</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>0.86519999999999997</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>0.86459999999999992</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>1.5107371594574315E-3</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>-8.7398321473430851E-4</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="3"/>
-        <v>0.49999999999999994</v>
-      </c>
-      <c r="C10">
+        <v>30.100000000000005</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="4"/>
-        <v>0.86602540378443871</v>
-      </c>
-      <c r="E10">
-        <f>A10+0.1</f>
-        <v>30.1</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="5"/>
-        <v>0.50151073715945738</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="6"/>
-        <v>0.8651514205697044</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0.86519999999999997</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
-        <v>0.86459999999999992</v>
-      </c>
-      <c r="L10">
-        <f>F10-B10</f>
-        <v>1.5107371594574315E-3</v>
-      </c>
-      <c r="M10">
-        <f>G10-C10</f>
-        <v>-8.7398321473430851E-4</v>
-      </c>
-      <c r="O10">
-        <f>DEGREES(ATAN2(G10,F10))</f>
-        <v>30.100000000000005</v>
-      </c>
-      <c r="P10">
-        <f>DEGREES(ATAN2(I10,F10))</f>
         <v>30.098604155521816</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>30.115852328171705</v>
       </c>
     </row>
@@ -20092,51 +20103,51 @@
         <v>45</v>
       </c>
       <c r="B11">
+        <f t="shared" si="8"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="9"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>45.1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="10"/>
+        <v>0.7083398377245288</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="11"/>
+        <v>0.705871570678681</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>0.70559999999999989</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="6"/>
+        <v>0.70559999999999989</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>1.2330565379813363E-3</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>-1.2352105078665687E-3</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="3"/>
-        <v>0.70710678118654746</v>
-      </c>
-      <c r="C11">
+        <v>45.099999999999994</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="4"/>
-        <v>0.70710678118654757</v>
-      </c>
-      <c r="E11">
-        <f>A11+0.1</f>
-        <v>45.1</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="5"/>
-        <v>0.7083398377245288</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="6"/>
-        <v>0.705871570678681</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>0.70559999999999989</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
-        <v>0.70559999999999989</v>
-      </c>
-      <c r="L11">
-        <f>F11-B11</f>
-        <v>1.2330565379813363E-3</v>
-      </c>
-      <c r="M11">
-        <f>G11-C11</f>
-        <v>-1.2352105078665687E-3</v>
-      </c>
-      <c r="O11">
-        <f>DEGREES(ATAN2(G11,F11))</f>
-        <v>45.099999999999994</v>
-      </c>
-      <c r="P11">
-        <f>DEGREES(ATAN2(I11,F11))</f>
         <v>45.111023777320867</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>45.111023777320867</v>
       </c>
     </row>
@@ -20145,51 +20156,51 @@
         <v>90</v>
       </c>
       <c r="B12">
-        <f>SIN(RADIANS(A12))</f>
+        <f t="shared" ref="B12:B17" si="12">SIN(RADIANS(A12))</f>
         <v>1</v>
       </c>
       <c r="C12">
-        <f>COS(RADIANS(A12))</f>
+        <f t="shared" ref="C12:C17" si="13">COS(RADIANS(A12))</f>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="E12">
-        <f>A12+0.1</f>
+        <f t="shared" si="0"/>
         <v>90.1</v>
       </c>
       <c r="F12" s="15">
-        <f>SIN(RADIANS(E12))</f>
+        <f t="shared" ref="F12:F17" si="14">SIN(RADIANS(E12))</f>
         <v>0.99999847691328769</v>
       </c>
       <c r="G12">
-        <f>COS(RADIANS(E12))</f>
+        <f t="shared" ref="G12:G17" si="15">COS(RADIANS(E12))</f>
         <v>-1.745328365898139E-3</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-1.8E-3</v>
       </c>
       <c r="J12">
+        <f t="shared" si="6"/>
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="L12" s="15">
         <f t="shared" si="1"/>
-        <v>-1.1999999999999999E-3</v>
-      </c>
-      <c r="L12" s="15">
-        <f>F12-B12</f>
         <v>-1.5230867123072755E-6</v>
       </c>
       <c r="M12">
-        <f>G12-C12</f>
+        <f t="shared" si="2"/>
         <v>-1.7453283658982002E-3</v>
       </c>
       <c r="O12">
-        <f>DEGREES(ATAN2(G12,F12))</f>
+        <f t="shared" si="3"/>
         <v>90.09999999999998</v>
       </c>
       <c r="P12">
-        <f>DEGREES(ATAN2(I12,F12))</f>
+        <f t="shared" si="4"/>
         <v>90.103132448820091</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>90.068755007133092</v>
       </c>
     </row>
@@ -20198,51 +20209,51 @@
         <v>135</v>
       </c>
       <c r="B13">
-        <f>SIN(RADIANS(A13))</f>
+        <f t="shared" si="12"/>
         <v>0.70710678118654757</v>
       </c>
       <c r="C13">
-        <f>COS(RADIANS(A13))</f>
+        <f t="shared" si="13"/>
         <v>-0.70710678118654746</v>
       </c>
       <c r="E13">
-        <f>A13+0.1</f>
+        <f t="shared" si="0"/>
         <v>135.1</v>
       </c>
       <c r="F13">
-        <f>SIN(RADIANS(E13))</f>
+        <f t="shared" si="14"/>
         <v>0.70587157067868112</v>
       </c>
       <c r="G13">
-        <f>COS(RADIANS(E13))</f>
+        <f t="shared" si="15"/>
         <v>-0.70833983772452869</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.7085999999999999</v>
       </c>
       <c r="J13">
+        <f t="shared" si="6"/>
+        <v>-0.70799999999999996</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="1"/>
-        <v>-0.70799999999999996</v>
-      </c>
-      <c r="L13">
-        <f>F13-B13</f>
         <v>-1.2352105078664577E-3</v>
       </c>
       <c r="M13">
-        <f>G13-C13</f>
+        <f t="shared" si="2"/>
         <v>-1.2330565379812253E-3</v>
       </c>
       <c r="O13">
-        <f>DEGREES(ATAN2(G13,F13))</f>
+        <f t="shared" si="3"/>
         <v>135.1</v>
       </c>
       <c r="P13">
-        <f>DEGREES(ATAN2(I13,F13))</f>
+        <f t="shared" si="4"/>
         <v>135.11051992430552</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>135.086252476895</v>
       </c>
     </row>
@@ -20251,51 +20262,51 @@
         <v>150</v>
       </c>
       <c r="B14">
-        <f>SIN(RADIANS(A14))</f>
+        <f t="shared" si="12"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="C14">
-        <f>COS(RADIANS(A14))</f>
+        <f t="shared" si="13"/>
         <v>-0.86602540378443871</v>
       </c>
       <c r="E14">
-        <f>A14+0.1</f>
+        <f t="shared" si="0"/>
         <v>150.1</v>
       </c>
       <c r="F14">
-        <f>SIN(RADIANS(E14))</f>
+        <f t="shared" si="14"/>
         <v>0.49848773975383037</v>
       </c>
       <c r="G14">
-        <f>COS(RADIANS(E14))</f>
+        <f t="shared" si="15"/>
         <v>-0.86689674893560276</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.86699999999999988</v>
       </c>
       <c r="J14">
+        <f t="shared" si="6"/>
+        <v>-0.86639999999999995</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="1"/>
-        <v>-0.86639999999999995</v>
-      </c>
-      <c r="L14">
-        <f>F14-B14</f>
         <v>-1.5122602461695722E-3</v>
       </c>
       <c r="M14">
-        <f>G14-C14</f>
+        <f t="shared" si="2"/>
         <v>-8.7134515116404909E-4</v>
       </c>
       <c r="O14">
-        <f>DEGREES(ATAN2(G14,F14))</f>
+        <f t="shared" si="3"/>
         <v>150.1</v>
       </c>
       <c r="P14">
-        <f>DEGREES(ATAN2(I14,F14))</f>
+        <f t="shared" si="4"/>
         <v>150.10294871486877</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>150.08580612060825</v>
       </c>
     </row>
@@ -20304,51 +20315,51 @@
         <v>160</v>
       </c>
       <c r="B15">
-        <f>SIN(RADIANS(A15))</f>
+        <f t="shared" si="12"/>
         <v>0.34202014332566888</v>
       </c>
       <c r="C15">
-        <f>COS(RADIANS(A15))</f>
+        <f t="shared" si="13"/>
         <v>-0.93969262078590832</v>
       </c>
       <c r="E15">
-        <f>A15+0.1</f>
+        <f t="shared" si="0"/>
         <v>160.1</v>
       </c>
       <c r="F15">
-        <f>SIN(RADIANS(E15))</f>
+        <f t="shared" si="14"/>
         <v>0.34037955021305039</v>
       </c>
       <c r="G15">
-        <f>COS(RADIANS(E15))</f>
+        <f t="shared" si="15"/>
         <v>-0.94028812701041886</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.94019999999999992</v>
       </c>
       <c r="J15">
+        <f t="shared" si="6"/>
+        <v>-0.94019999999999992</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="1"/>
-        <v>-0.94019999999999992</v>
-      </c>
-      <c r="L15">
-        <f>F15-B15</f>
         <v>-1.6405931126184936E-3</v>
       </c>
       <c r="M15">
-        <f>G15-C15</f>
+        <f t="shared" si="2"/>
         <v>-5.9550622451054469E-4</v>
       </c>
       <c r="O15">
-        <f>DEGREES(ATAN2(G15,F15))</f>
+        <f t="shared" si="3"/>
         <v>160.1</v>
       </c>
       <c r="P15">
-        <f>DEGREES(ATAN2(I15,F15))</f>
+        <f t="shared" si="4"/>
         <v>160.09828117714778</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>160.09828117714778</v>
       </c>
     </row>
@@ -20357,51 +20368,51 @@
         <v>170</v>
       </c>
       <c r="B16">
-        <f>SIN(RADIANS(A16))</f>
+        <f t="shared" si="12"/>
         <v>0.17364817766693028</v>
       </c>
       <c r="C16">
-        <f>COS(RADIANS(A16))</f>
+        <f t="shared" si="13"/>
         <v>-0.98480775301220802</v>
       </c>
       <c r="E16">
-        <f>A16+0.1</f>
+        <f t="shared" si="0"/>
         <v>170.1</v>
       </c>
       <c r="F16">
-        <f>SIN(RADIANS(E16))</f>
+        <f t="shared" si="14"/>
         <v>0.17192910027940958</v>
       </c>
       <c r="G16">
-        <f>COS(RADIANS(E16))</f>
+        <f t="shared" si="15"/>
         <v>-0.98510932615477387</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.98519999999999996</v>
       </c>
       <c r="J16">
+        <f t="shared" si="6"/>
+        <v>-0.98459999999999992</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="1"/>
-        <v>-0.98459999999999992</v>
-      </c>
-      <c r="L16">
-        <f>F16-B16</f>
         <v>-1.7190773875206955E-3</v>
       </c>
       <c r="M16">
-        <f>G16-C16</f>
+        <f t="shared" si="2"/>
         <v>-3.0157314256584744E-4</v>
       </c>
       <c r="O16">
-        <f>DEGREES(ATAN2(G16,F16))</f>
+        <f t="shared" si="3"/>
         <v>170.1</v>
       </c>
       <c r="P16">
-        <f>DEGREES(ATAN2(I16,F16))</f>
+        <f t="shared" si="4"/>
         <v>170.10089313120864</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>170.09498020526482</v>
       </c>
     </row>
@@ -20410,51 +20421,51 @@
         <v>175</v>
       </c>
       <c r="B17">
-        <f>SIN(RADIANS(A17))</f>
+        <f t="shared" si="12"/>
         <v>8.7155742747658194E-2</v>
       </c>
       <c r="C17">
-        <f>COS(RADIANS(A17))</f>
+        <f t="shared" si="13"/>
         <v>-0.99619469809174555</v>
       </c>
       <c r="E17">
-        <f>A17+0.1</f>
+        <f t="shared" si="0"/>
         <v>175.1</v>
       </c>
       <c r="F17">
-        <f>SIN(RADIANS(E17))</f>
+        <f t="shared" si="14"/>
         <v>8.5416923137367595E-2</v>
       </c>
       <c r="G17">
-        <f>COS(RADIANS(E17))</f>
+        <f t="shared" si="15"/>
         <v>-0.99634529619090639</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.99659999999999993</v>
       </c>
       <c r="J17">
+        <f t="shared" si="6"/>
+        <v>-0.99599999999999989</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="1"/>
-        <v>-0.99599999999999989</v>
-      </c>
-      <c r="L17">
-        <f>F17-B17</f>
         <v>-1.7388196102905984E-3</v>
       </c>
       <c r="M17" s="16">
-        <f>G17-C17</f>
+        <f t="shared" si="2"/>
         <v>-1.5059809916084799E-4</v>
       </c>
       <c r="O17">
-        <f>DEGREES(ATAN2(G17,F17))</f>
+        <f t="shared" si="3"/>
         <v>175.1</v>
       </c>
       <c r="P17">
-        <f>DEGREES(ATAN2(I17,F17))</f>
+        <f t="shared" si="4"/>
         <v>175.10124621162274</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>175.09830952878136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added low power functionality
</commit_message>
<xml_diff>
--- a/Encoder Characteristics.xlsx
+++ b/Encoder Characteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pauld\Programming\NN54\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD26F578-78E7-4E0D-AB56-A46F84BC945D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F7CAC2-65A9-439D-B555-C5AA830F6443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encoder Error" sheetId="1" r:id="rId1"/>
@@ -415,13 +415,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:K607"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="163" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C10" zoomScale="163" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -828,7 +828,7 @@
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
-      <c r="H5" s="21">
+      <c r="H5" s="19">
         <v>50000000</v>
       </c>
       <c r="I5">
@@ -13506,33 +13506,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20"/>
+      <c r="D2" s="21"/>
       <c r="E2">
         <v>100</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" s="21"/>
       <c r="I2">
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
@@ -18199,10 +18199,10 @@
       <c r="AA107" s="8"/>
     </row>
     <row r="108" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B108" s="19" t="s">
+      <c r="B108" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C108" s="19"/>
+      <c r="C108" s="20"/>
       <c r="D108" s="6">
         <v>0</v>
       </c>
@@ -19260,8 +19260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3BDFF7-A03C-4436-BDC7-9DE4C8404CC4}">
   <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="E3" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -19275,11 +19275,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
       <c r="J1" s="12"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -19292,7 +19292,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="18">
-        <v>9.6999999999999993</v>
+        <v>9.68</v>
       </c>
       <c r="I4" s="18">
         <v>0.41399999999999998</v>
@@ -19303,10 +19303,10 @@
         <v>19</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>1.66</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>1.66</v>
       </c>
       <c r="L5">
         <v>3500</v>
@@ -19317,10 +19317,10 @@
         <v>20</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2.56</v>
       </c>
       <c r="I6" s="18">
-        <v>3</v>
+        <v>2.56</v>
       </c>
       <c r="J6" s="17"/>
     </row>
@@ -19334,6 +19334,14 @@
       <c r="I7">
         <v>9</v>
       </c>
+      <c r="J7">
+        <f>SUM(H4:H6)</f>
+        <v>13.9</v>
+      </c>
+      <c r="K7">
+        <f>K10-SUM(H5:H6)</f>
+        <v>1.2999999999999998</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
@@ -19352,11 +19360,16 @@
       </c>
       <c r="H9">
         <f>SUM(H4:H8)</f>
-        <v>38.700000000000003</v>
+        <v>36.9</v>
       </c>
       <c r="I9">
         <f>SUM(I4:I8)</f>
-        <v>15.414</v>
+        <v>13.634</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>5.52</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -19365,11 +19378,11 @@
       </c>
       <c r="H11">
         <f>L5/H9</f>
-        <v>90.439276485788113</v>
+        <v>94.850948509485093</v>
       </c>
       <c r="I11">
         <f>L5/I9</f>
-        <v>227.06630336058129</v>
+        <v>256.71116326829986</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -19378,11 +19391,11 @@
       </c>
       <c r="H12">
         <f>H11/4</f>
-        <v>22.609819121447028</v>
+        <v>23.712737127371273</v>
       </c>
       <c r="I12">
         <f>I11/4</f>
-        <v>56.766575840145322</v>
+        <v>64.177790817074964</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -19499,10 +19512,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="21"/>
       <c r="H4">
         <v>72000000</v>
       </c>

</xml_diff>

<commit_message>
Finished rev 1 device
</commit_message>
<xml_diff>
--- a/Encoder Characteristics.xlsx
+++ b/Encoder Characteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pauld\Programming\NN54\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F503C8E-1233-4B27-9615-B34B9C2E3892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BBE57E-6C77-469D-990B-0AE63891370E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encoder Error" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>Number of measurments</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Hipotenusa</t>
   </si>
   <si>
-    <t>Punto Circulo Unit</t>
-  </si>
-  <si>
     <t>dt</t>
   </si>
   <si>
@@ -144,16 +141,10 @@
     <t>dps</t>
   </si>
   <si>
-    <t>dps satur</t>
-  </si>
-  <si>
     <t>dA</t>
   </si>
   <si>
     <t>dA/dt</t>
-  </si>
-  <si>
-    <t>dps/dt</t>
   </si>
   <si>
     <t>Vel</t>
@@ -305,6 +296,12 @@
   <si>
     <t>Atan Corr T</t>
   </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>init length</t>
+  </si>
 </sst>
 </file>
 
@@ -377,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -418,12 +415,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:K607"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" zoomScale="163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -814,16 +812,16 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="I4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
@@ -13484,12 +13482,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11AFDFB-30EA-4EFD-BE21-A5C5DCB81B95}">
   <dimension ref="B2:AA147"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="I123" sqref="I123"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N76" sqref="G76:N77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
@@ -18134,9 +18133,6 @@
       <c r="U105" s="9"/>
     </row>
     <row r="106" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C106">
-        <v>0.01</v>
-      </c>
       <c r="F106" s="5" t="s">
         <v>31</v>
       </c>
@@ -18147,15 +18143,15 @@
         <v>29</v>
       </c>
       <c r="L106" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="N106" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="U106" s="9"/>
       <c r="V106" s="9"/>
     </row>
     <row r="107" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>87</v>
+      </c>
       <c r="E107" s="5" t="s">
         <v>14</v>
       </c>
@@ -18169,22 +18165,22 @@
         <v>13</v>
       </c>
       <c r="I107" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J107" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K107" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L107" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K107" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L107" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="M107" s="5" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="N107" s="5" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="Q107" s="11"/>
       <c r="R107" s="11"/>
@@ -18199,27 +18195,25 @@
       <c r="AA107" s="8"/>
     </row>
     <row r="108" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B108" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C108" s="20"/>
+      <c r="B108" s="22"/>
+      <c r="C108" s="22"/>
       <c r="D108" s="6">
         <v>0</v>
       </c>
       <c r="E108" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108" s="7">
-        <f>$C$106+($I$2*D108)</f>
-        <v>0.01</v>
+        <f>$B$111+($I$2*D108)</f>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="G108" s="7">
         <f>COS(RADIANS(E108))*F108</f>
-        <v>0.01</v>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H108" s="7">
         <f t="shared" ref="H108:H123" si="45">SIN(RADIANS(E108))*F108</f>
-        <v>0</v>
+        <v>1.466002140731815E-3</v>
       </c>
       <c r="J108" s="5"/>
       <c r="K108" s="5"/>
@@ -18241,48 +18235,44 @@
         <v>1</v>
       </c>
       <c r="E109">
-        <f t="shared" ref="E109:E123" si="46">DEGREES(ACOS(G109/F109) )</f>
-        <v>41.731817039793761</v>
+        <f>DEGREES(ACOS(G109/F109) )</f>
+        <v>16.064246027615003</v>
       </c>
       <c r="F109" s="5">
-        <f t="shared" ref="F109:F123" si="47">$C$106+($I$2*D109)</f>
-        <v>1.34E-2</v>
+        <f>$B$111+($I$2*D109)</f>
+        <v>8.7400000000000005E-2</v>
       </c>
       <c r="G109" s="5">
         <f>G108</f>
-        <v>0.01</v>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H109" s="5">
         <f t="shared" si="45"/>
-        <v>8.9196412483911035E-3</v>
+        <v>2.4184895333175027E-2</v>
       </c>
       <c r="I109">
         <f>E109-E108</f>
-        <v>41.731817039793761</v>
+        <v>15.064246027615003</v>
       </c>
       <c r="J109">
-        <f t="shared" ref="J109:J123" si="48">H109-H108</f>
-        <v>8.9196412483911035E-3</v>
+        <f t="shared" ref="J109:J123" si="46">H109-H108</f>
+        <v>2.2718893192443211E-2</v>
       </c>
       <c r="K109">
-        <f>J109/$C$113</f>
-        <v>1.4866068747318507E-3</v>
+        <f>J109/$C$111</f>
+        <v>3.7864821987405352E-3</v>
       </c>
       <c r="L109">
         <f>(E109-E108)/K109</f>
-        <v>28071.857966700987</v>
+        <v>3978.4277957587369</v>
       </c>
       <c r="M109">
-        <f t="shared" ref="M109:M117" si="49">IF(L109&gt;2000,2000,L109)</f>
-        <v>2000</v>
+        <f>L109/360</f>
+        <v>11.051188321552047</v>
       </c>
       <c r="N109">
-        <f t="shared" ref="N109:N117" si="50">M109*K109</f>
-        <v>2.9732137494637012</v>
-      </c>
-      <c r="O109">
-        <f>E108+N109</f>
-        <v>2.9732137494637012</v>
+        <f>M109*60</f>
+        <v>663.07129929312282</v>
       </c>
       <c r="Q109" s="11"/>
       <c r="R109" s="8"/>
@@ -18297,52 +18287,54 @@
       <c r="AA109" s="8"/>
     </row>
     <row r="110" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B110" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="D110">
         <v>2</v>
       </c>
       <c r="E110">
-        <f t="shared" si="46"/>
-        <v>53.470392770264972</v>
+        <f t="shared" ref="E109:E123" si="47">DEGREES(ACOS(G110/F110) )</f>
+        <v>22.336283890705477</v>
       </c>
       <c r="F110" s="5">
-        <f t="shared" si="47"/>
-        <v>1.6799999999999999E-2</v>
+        <f>$B$111+($I$2*D110)</f>
+        <v>9.0800000000000006E-2</v>
       </c>
       <c r="G110" s="5">
         <f>G109</f>
-        <v>0.01</v>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H110" s="5">
         <f t="shared" si="45"/>
-        <v>1.3499629624548964E-2</v>
+        <v>3.450781306134354E-2</v>
       </c>
       <c r="I110">
-        <f t="shared" ref="I110:I122" si="51">E110-E109</f>
-        <v>11.738575730471212</v>
+        <f t="shared" ref="I110:I122" si="48">E110-E109</f>
+        <v>6.2720378630904747</v>
       </c>
       <c r="J110">
-        <f t="shared" si="48"/>
-        <v>4.5799883761578602E-3</v>
+        <f t="shared" si="46"/>
+        <v>1.0322917728168512E-2</v>
       </c>
       <c r="K110">
-        <f t="shared" ref="K110:K117" si="52">J110/$C$113</f>
-        <v>7.6333139602631007E-4</v>
+        <f>J110/$C$111</f>
+        <v>1.7204862880280853E-3</v>
       </c>
       <c r="L110">
-        <f t="shared" ref="L110:L117" si="53">(E110-E109)/K110</f>
-        <v>15378.085837395078</v>
+        <f t="shared" ref="L110:L123" si="49">(E110-E109)/K110</f>
+        <v>3645.5029643270773</v>
       </c>
       <c r="M110">
-        <f t="shared" si="49"/>
-        <v>2000</v>
+        <f t="shared" ref="M110:M123" si="50">L110/360</f>
+        <v>10.12639712313077</v>
       </c>
       <c r="N110">
-        <f t="shared" si="50"/>
-        <v>1.5266627920526201</v>
-      </c>
-      <c r="O110">
-        <f t="shared" ref="O110:O117" si="54">O109+N110</f>
-        <v>4.4998765415163211</v>
+        <f t="shared" ref="N110:N123" si="51">M110*60</f>
+        <v>607.58382738784621</v>
       </c>
       <c r="Q110" s="11"/>
       <c r="R110" s="8"/>
@@ -18357,52 +18349,54 @@
       <c r="AA110" s="8"/>
     </row>
     <row r="111" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B111" s="20">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="C111" s="20">
+        <v>6</v>
+      </c>
       <c r="D111">
         <v>3</v>
       </c>
       <c r="E111">
-        <f t="shared" si="46"/>
-        <v>60.326985197525957</v>
+        <f t="shared" si="47"/>
+        <v>26.927037168594467</v>
       </c>
       <c r="F111" s="5">
-        <f t="shared" si="47"/>
-        <v>2.0199999999999999E-2</v>
+        <f>$B$111+($I$2*D111)</f>
+        <v>9.4200000000000006E-2</v>
       </c>
       <c r="G111" s="5">
-        <f t="shared" ref="G111:G117" si="55">G110</f>
-        <v>0.01</v>
+        <f t="shared" ref="G111:G117" si="52">G110</f>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H111" s="5">
         <f t="shared" si="45"/>
-        <v>1.7551068343551055E-2</v>
+        <v>4.2658986887602356E-2</v>
       </c>
       <c r="I111">
+        <f t="shared" si="48"/>
+        <v>4.5907532778889895</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="46"/>
+        <v>8.151173826258816E-3</v>
+      </c>
+      <c r="K111">
+        <f>J111/$C$111</f>
+        <v>1.358528971043136E-3</v>
+      </c>
+      <c r="L111">
+        <f t="shared" si="49"/>
+        <v>3379.2089647996354</v>
+      </c>
+      <c r="M111">
+        <f t="shared" si="50"/>
+        <v>9.3866915688878763</v>
+      </c>
+      <c r="N111">
         <f t="shared" si="51"/>
-        <v>6.8565924272609848</v>
-      </c>
-      <c r="J111">
-        <f t="shared" si="48"/>
-        <v>4.0514387190020915E-3</v>
-      </c>
-      <c r="K111">
-        <f t="shared" si="52"/>
-        <v>6.7523978650034858E-4</v>
-      </c>
-      <c r="L111">
-        <f t="shared" si="53"/>
-        <v>10154.307498374053</v>
-      </c>
-      <c r="M111">
-        <f t="shared" si="49"/>
-        <v>2000</v>
-      </c>
-      <c r="N111">
-        <f t="shared" si="50"/>
-        <v>1.3504795730006971</v>
-      </c>
-      <c r="O111">
-        <f t="shared" si="54"/>
-        <v>5.8503561145170178</v>
+        <v>563.2014941332726</v>
       </c>
       <c r="Q111" s="11"/>
       <c r="R111" s="8"/>
@@ -18417,55 +18411,48 @@
       <c r="AA111" s="8"/>
     </row>
     <row r="112" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
-        <v>40</v>
-      </c>
       <c r="D112">
         <v>4</v>
       </c>
       <c r="E112">
-        <f t="shared" si="46"/>
-        <v>64.929772050657689</v>
+        <f t="shared" si="47"/>
+        <v>30.624457670866033</v>
       </c>
       <c r="F112" s="5">
-        <f t="shared" si="47"/>
-        <v>2.3599999999999999E-2</v>
+        <f>$B$111+($I$2*D112)</f>
+        <v>9.7600000000000006E-2</v>
       </c>
       <c r="G112" s="5">
-        <f t="shared" si="55"/>
-        <v>0.01</v>
+        <f t="shared" si="52"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H112" s="5">
         <f t="shared" si="45"/>
-        <v>2.1376622745419821E-2</v>
+        <v>4.9718298062952943E-2</v>
       </c>
       <c r="I112">
+        <f t="shared" si="48"/>
+        <v>3.6974205022715658</v>
+      </c>
+      <c r="J112">
+        <f t="shared" si="46"/>
+        <v>7.0593111753505869E-3</v>
+      </c>
+      <c r="K112">
+        <f>J112/$C$111</f>
+        <v>1.1765518625584312E-3</v>
+      </c>
+      <c r="L112">
+        <f t="shared" si="49"/>
+        <v>3142.5903268143784</v>
+      </c>
+      <c r="M112">
+        <f t="shared" si="50"/>
+        <v>8.7294175744843852</v>
+      </c>
+      <c r="N112">
         <f t="shared" si="51"/>
-        <v>4.6027868531317324</v>
-      </c>
-      <c r="J112">
-        <f t="shared" si="48"/>
-        <v>3.8255544018687658E-3</v>
-      </c>
-      <c r="K112">
-        <f t="shared" si="52"/>
-        <v>6.3759240031146093E-4</v>
-      </c>
-      <c r="L112">
-        <f t="shared" si="53"/>
-        <v>7219.0114732912316</v>
-      </c>
-      <c r="M112">
-        <f t="shared" si="49"/>
-        <v>2000</v>
-      </c>
-      <c r="N112">
-        <f t="shared" si="50"/>
-        <v>1.2751848006229218</v>
-      </c>
-      <c r="O112">
-        <f t="shared" si="54"/>
-        <v>7.1255409151399398</v>
+        <v>523.7650544690631</v>
       </c>
       <c r="Q112" s="11"/>
       <c r="R112" s="8"/>
@@ -18480,55 +18467,54 @@
       <c r="AA112" s="8"/>
     </row>
     <row r="113" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>75</v>
+      </c>
       <c r="C113">
-        <v>6</v>
+        <v>500</v>
       </c>
       <c r="D113">
         <v>5</v>
       </c>
       <c r="E113">
         <f>DEGREES(ACOS(G113/F113) )</f>
-        <v>68.261539208479505</v>
+        <v>33.741038359886566</v>
       </c>
       <c r="F113" s="5">
-        <f t="shared" si="47"/>
-        <v>2.6999999999999996E-2</v>
+        <f>$B$111+($I$2*D113)</f>
+        <v>0.10100000000000001</v>
       </c>
       <c r="G113" s="5">
-        <f t="shared" si="55"/>
-        <v>0.01</v>
+        <f t="shared" si="52"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H113" s="5">
         <f t="shared" si="45"/>
-        <v>2.5079872407968898E-2</v>
+        <v>5.6099457771681099E-2</v>
       </c>
       <c r="I113">
+        <f t="shared" si="48"/>
+        <v>3.1165806890205339</v>
+      </c>
+      <c r="J113">
+        <f t="shared" si="46"/>
+        <v>6.3811597087281569E-3</v>
+      </c>
+      <c r="K113">
+        <f>J113/$C$111</f>
+        <v>1.0635266181213594E-3</v>
+      </c>
+      <c r="L113">
+        <f t="shared" si="49"/>
+        <v>2930.420956013063</v>
+      </c>
+      <c r="M113">
+        <f t="shared" si="50"/>
+        <v>8.140058211147398</v>
+      </c>
+      <c r="N113">
         <f t="shared" si="51"/>
-        <v>3.3317671578218153</v>
-      </c>
-      <c r="J113">
-        <f t="shared" si="48"/>
-        <v>3.7032496625490768E-3</v>
-      </c>
-      <c r="K113">
-        <f t="shared" si="52"/>
-        <v>6.1720827709151277E-4</v>
-      </c>
-      <c r="L113">
-        <f t="shared" si="53"/>
-        <v>5398.1245577622385</v>
-      </c>
-      <c r="M113">
-        <f t="shared" si="49"/>
-        <v>2000</v>
-      </c>
-      <c r="N113">
-        <f t="shared" si="50"/>
-        <v>1.2344165541830256</v>
-      </c>
-      <c r="O113">
-        <f t="shared" si="54"/>
-        <v>8.3599574693229659</v>
+        <v>488.40349266884391</v>
       </c>
       <c r="Q113" s="11"/>
       <c r="R113" s="8"/>
@@ -18543,52 +18529,54 @@
       <c r="AA113" s="8"/>
     </row>
     <row r="114" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>73</v>
+      </c>
+      <c r="C114">
+        <v>100</v>
+      </c>
       <c r="D114">
         <v>6</v>
       </c>
       <c r="E114">
-        <f t="shared" si="46"/>
-        <v>70.795102502870591</v>
+        <f t="shared" si="47"/>
+        <v>36.44040124394018</v>
       </c>
       <c r="F114" s="5">
-        <f t="shared" si="47"/>
-        <v>3.0399999999999996E-2</v>
+        <f>$B$111+($I$2*D114)</f>
+        <v>0.10440000000000001</v>
       </c>
       <c r="G114" s="5">
-        <f t="shared" si="55"/>
-        <v>0.01</v>
+        <f t="shared" si="52"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H114" s="5">
         <f t="shared" si="45"/>
-        <v>2.8708186985596976E-2</v>
+        <v>6.201216946919879E-2</v>
       </c>
       <c r="I114">
+        <f t="shared" si="48"/>
+        <v>2.6993628840536132</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="46"/>
+        <v>5.9127116975176905E-3</v>
+      </c>
+      <c r="K114">
+        <f>J114/$C$111</f>
+        <v>9.8545194958628182E-4</v>
+      </c>
+      <c r="L114">
+        <f t="shared" si="49"/>
+        <v>2739.2130942425711</v>
+      </c>
+      <c r="M114">
+        <f t="shared" si="50"/>
+        <v>7.6089252617849192</v>
+      </c>
+      <c r="N114">
         <f t="shared" si="51"/>
-        <v>2.5335632943910866</v>
-      </c>
-      <c r="J114">
-        <f t="shared" si="48"/>
-        <v>3.6283145776280779E-3</v>
-      </c>
-      <c r="K114">
-        <f t="shared" si="52"/>
-        <v>6.0471909627134634E-4</v>
-      </c>
-      <c r="L114">
-        <f t="shared" si="53"/>
-        <v>4189.6531960258117</v>
-      </c>
-      <c r="M114">
-        <f t="shared" si="49"/>
-        <v>2000</v>
-      </c>
-      <c r="N114">
-        <f t="shared" si="50"/>
-        <v>1.2094381925426927</v>
-      </c>
-      <c r="O114">
-        <f t="shared" si="54"/>
-        <v>9.5693956618656593</v>
+        <v>456.53551570709516</v>
       </c>
       <c r="Q114" s="8"/>
       <c r="R114" s="8"/>
@@ -18603,52 +18591,55 @@
       <c r="AA114" s="8"/>
     </row>
     <row r="115" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B115" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C115">
+        <f>1/(2*3.1416*C114*C113)</f>
+        <v>3.1830914183855364E-6</v>
+      </c>
       <c r="D115">
         <v>7</v>
       </c>
       <c r="E115">
-        <f t="shared" si="46"/>
-        <v>72.791006778084139</v>
+        <f t="shared" si="47"/>
+        <v>38.821562103911269</v>
       </c>
       <c r="F115" s="5">
-        <f t="shared" si="47"/>
-        <v>3.3799999999999997E-2</v>
+        <f>$B$111+($I$2*D115)</f>
+        <v>0.10780000000000001</v>
       </c>
       <c r="G115" s="5">
-        <f t="shared" si="55"/>
-        <v>0.01</v>
+        <f t="shared" si="52"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H115" s="5">
         <f t="shared" si="45"/>
-        <v>3.2286839424136883E-2</v>
+        <v>6.7579502530550117E-2</v>
       </c>
       <c r="I115">
+        <f t="shared" si="48"/>
+        <v>2.3811608599710894</v>
+      </c>
+      <c r="J115">
+        <f t="shared" si="46"/>
+        <v>5.5673330613513275E-3</v>
+      </c>
+      <c r="K115">
+        <f>J115/$C$111</f>
+        <v>9.2788884355855458E-4</v>
+      </c>
+      <c r="L115">
+        <f t="shared" si="49"/>
+        <v>2566.2134818208165</v>
+      </c>
+      <c r="M115">
+        <f t="shared" si="50"/>
+        <v>7.1283707828356011</v>
+      </c>
+      <c r="N115">
         <f t="shared" si="51"/>
-        <v>1.9959042752135474</v>
-      </c>
-      <c r="J115">
-        <f t="shared" si="48"/>
-        <v>3.5786524385399074E-3</v>
-      </c>
-      <c r="K115">
-        <f t="shared" si="52"/>
-        <v>5.9644207308998456E-4</v>
-      </c>
-      <c r="L115">
-        <f t="shared" si="53"/>
-        <v>3346.3505766341664</v>
-      </c>
-      <c r="M115">
-        <f t="shared" si="49"/>
-        <v>2000</v>
-      </c>
-      <c r="N115">
-        <f t="shared" si="50"/>
-        <v>1.1928841461799691</v>
-      </c>
-      <c r="O115">
-        <f t="shared" si="54"/>
-        <v>10.762279808045628</v>
+        <v>427.70224697013606</v>
       </c>
       <c r="Q115" s="11"/>
       <c r="R115" s="11"/>
@@ -18663,52 +18654,49 @@
       <c r="AA115" s="8"/>
     </row>
     <row r="116" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="C116" s="4"/>
       <c r="D116">
         <v>8</v>
       </c>
       <c r="E116">
-        <f t="shared" si="46"/>
-        <v>74.406104259530906</v>
+        <f t="shared" si="47"/>
+        <v>40.950103091476691</v>
       </c>
       <c r="F116" s="5">
-        <f t="shared" si="47"/>
-        <v>3.7199999999999997E-2</v>
+        <f>$B$111+($I$2*D116)</f>
+        <v>0.11120000000000001</v>
       </c>
       <c r="G116" s="5">
-        <f t="shared" si="55"/>
-        <v>0.01</v>
+        <f t="shared" si="52"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H116" s="5">
         <f t="shared" si="45"/>
-        <v>3.5830713082493908E-2</v>
+        <v>7.2880650122488816E-2</v>
       </c>
       <c r="I116">
+        <f t="shared" si="48"/>
+        <v>2.1285409875654224</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="46"/>
+        <v>5.3011475919386986E-3</v>
+      </c>
+      <c r="K116">
+        <f>J116/$C$111</f>
+        <v>8.8352459865644972E-4</v>
+      </c>
+      <c r="L116">
+        <f t="shared" si="49"/>
+        <v>2409.1473975962108</v>
+      </c>
+      <c r="M116">
+        <f t="shared" si="50"/>
+        <v>6.6920761044339185</v>
+      </c>
+      <c r="N116">
         <f t="shared" si="51"/>
-        <v>1.6150974814467673</v>
-      </c>
-      <c r="J116">
-        <f t="shared" si="48"/>
-        <v>3.5438736583570246E-3</v>
-      </c>
-      <c r="K116">
-        <f t="shared" si="52"/>
-        <v>5.9064560972617081E-4</v>
-      </c>
-      <c r="L116">
-        <f t="shared" si="53"/>
-        <v>2734.4611639381228</v>
-      </c>
-      <c r="M116">
-        <f t="shared" si="49"/>
-        <v>2000</v>
-      </c>
-      <c r="N116">
-        <f t="shared" si="50"/>
-        <v>1.1812912194523415</v>
-      </c>
-      <c r="O116">
-        <f t="shared" si="54"/>
-        <v>11.943571027497971</v>
+        <v>401.52456626603509</v>
       </c>
       <c r="Q116" s="11"/>
       <c r="R116" s="8"/>
@@ -18723,52 +18711,55 @@
       <c r="AA116" s="8"/>
     </row>
     <row r="117" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>71</v>
+      </c>
+      <c r="C117">
+        <f>M109</f>
+        <v>11.051188321552047</v>
+      </c>
       <c r="D117">
         <v>9</v>
       </c>
       <c r="E117">
-        <f t="shared" si="46"/>
-        <v>75.741006958527521</v>
+        <f t="shared" si="47"/>
+        <v>42.872237324946603</v>
       </c>
       <c r="F117" s="5">
-        <f t="shared" si="47"/>
-        <v>4.0599999999999997E-2</v>
+        <f>$B$111+($I$2*D117)</f>
+        <v>0.11460000000000001</v>
       </c>
       <c r="G117" s="5">
-        <f t="shared" si="55"/>
-        <v>0.01</v>
+        <f t="shared" si="52"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H117" s="5">
         <f t="shared" si="45"/>
-        <v>3.9349205836967029E-2</v>
+        <v>7.7969924729196921E-2</v>
       </c>
       <c r="I117">
+        <f t="shared" si="48"/>
+        <v>1.9221342334699116</v>
+      </c>
+      <c r="J117">
+        <f t="shared" si="46"/>
+        <v>5.0892746067081052E-3</v>
+      </c>
+      <c r="K117">
+        <f>J117/$C$111</f>
+        <v>8.4821243445135086E-4</v>
+      </c>
+      <c r="L117">
+        <f t="shared" si="49"/>
+        <v>2266.1000421589029</v>
+      </c>
+      <c r="M117">
+        <f t="shared" si="50"/>
+        <v>6.2947223393302858</v>
+      </c>
+      <c r="N117">
         <f t="shared" si="51"/>
-        <v>1.3349026989966148</v>
-      </c>
-      <c r="J117">
-        <f t="shared" si="48"/>
-        <v>3.5184927544731209E-3</v>
-      </c>
-      <c r="K117">
-        <f t="shared" si="52"/>
-        <v>5.8641545907885345E-4</v>
-      </c>
-      <c r="L117">
-        <f t="shared" si="53"/>
-        <v>2276.377060545934</v>
-      </c>
-      <c r="M117">
-        <f t="shared" si="49"/>
-        <v>2000</v>
-      </c>
-      <c r="N117">
-        <f t="shared" si="50"/>
-        <v>1.172830918157707</v>
-      </c>
-      <c r="O117">
-        <f t="shared" si="54"/>
-        <v>13.116401945655678</v>
+        <v>377.68334035981712</v>
       </c>
       <c r="Q117" s="11"/>
       <c r="R117" s="8"/>
@@ -18783,39 +18774,55 @@
       <c r="AA117" s="8"/>
     </row>
     <row r="118" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
-        <v>34</v>
-      </c>
-      <c r="C118">
-        <f>H109-H108</f>
-        <v>8.9196412483911035E-3</v>
+      <c r="B118" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C118" s="13">
+        <f>1/(2*3.1416*C117*C115)</f>
+        <v>4524.4003219536035</v>
       </c>
       <c r="D118">
         <v>10</v>
       </c>
       <c r="E118">
-        <f t="shared" si="46"/>
-        <v>76.863441213055154</v>
+        <f t="shared" si="47"/>
+        <v>44.622032603569437</v>
       </c>
       <c r="F118" s="5">
-        <f t="shared" si="47"/>
-        <v>4.3999999999999997E-2</v>
+        <f>$B$111+($I$2*D118)</f>
+        <v>0.11799999999999999</v>
       </c>
       <c r="G118" s="5">
-        <f t="shared" ref="G118:G123" si="56">G117</f>
-        <v>0.01</v>
+        <f t="shared" ref="G118:G123" si="53">G117</f>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H118" s="5">
         <f>SIN(RADIANS(E118))*F118</f>
-        <v>4.28485705712571E-2</v>
+        <v>8.2886362945159026E-2</v>
       </c>
       <c r="I118">
+        <f t="shared" si="48"/>
+        <v>1.7497952786228339</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="46"/>
+        <v>4.9164382159621045E-3</v>
+      </c>
+      <c r="K118">
+        <f>J118/$C$111</f>
+        <v>8.1940636932701738E-4</v>
+      </c>
+      <c r="L118">
+        <f t="shared" si="49"/>
+        <v>2135.4426132420103</v>
+      </c>
+      <c r="M118">
+        <f t="shared" si="50"/>
+        <v>5.9317850367833618</v>
+      </c>
+      <c r="N118">
         <f t="shared" si="51"/>
-        <v>1.1224342545276329</v>
-      </c>
-      <c r="J118">
-        <f t="shared" si="48"/>
-        <v>3.4993647342900711E-3</v>
+        <v>355.90710220700169</v>
       </c>
       <c r="Q118" s="11"/>
       <c r="R118" s="8"/>
@@ -18830,39 +18837,48 @@
       <c r="AA118" s="8"/>
     </row>
     <row r="119" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>33</v>
-      </c>
-      <c r="C119">
-        <f>C118/C113</f>
-        <v>1.4866068747318507E-3</v>
-      </c>
       <c r="D119">
         <v>11</v>
       </c>
       <c r="E119">
-        <f t="shared" si="46"/>
-        <v>77.820770023802041</v>
+        <f t="shared" si="47"/>
+        <v>46.225480244483315</v>
       </c>
       <c r="F119" s="5">
-        <f t="shared" si="47"/>
-        <v>4.7399999999999998E-2</v>
+        <f>$B$111+($I$2*D119)</f>
+        <v>0.12140000000000001</v>
       </c>
       <c r="G119" s="5">
-        <f t="shared" si="56"/>
-        <v>0.01</v>
+        <f t="shared" si="53"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H119" s="5">
         <f t="shared" si="45"/>
-        <v>4.6333141486413369E-2</v>
+        <v>8.7659050658084547E-2</v>
       </c>
       <c r="I119">
+        <f t="shared" si="48"/>
+        <v>1.6034476409138776</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="46"/>
+        <v>4.7726877129255219E-3</v>
+      </c>
+      <c r="K119">
+        <f>J119/$C$111</f>
+        <v>7.9544795215425368E-4</v>
+      </c>
+      <c r="L119">
+        <f t="shared" si="49"/>
+        <v>2015.7794568096847</v>
+      </c>
+      <c r="M119">
+        <f t="shared" si="50"/>
+        <v>5.5993873800269016</v>
+      </c>
+      <c r="N119">
         <f t="shared" si="51"/>
-        <v>0.95732881074688692</v>
-      </c>
-      <c r="J119">
-        <f t="shared" si="48"/>
-        <v>3.4845709151562695E-3</v>
+        <v>335.96324280161411</v>
       </c>
       <c r="Q119" s="11"/>
       <c r="R119" s="8"/>
@@ -18877,39 +18893,54 @@
       <c r="AA119" s="8"/>
     </row>
     <row r="120" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>35</v>
+      <c r="B120" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="C120">
-        <f>(E117-E108)/C119</f>
-        <v>50948.914770886848</v>
+        <v>2.8</v>
       </c>
       <c r="D120">
         <v>12</v>
       </c>
       <c r="E120">
-        <f t="shared" si="46"/>
-        <v>78.647161243661103</v>
+        <f t="shared" si="47"/>
+        <v>47.702951616830354</v>
       </c>
       <c r="F120" s="5">
-        <f t="shared" si="47"/>
-        <v>5.0799999999999998E-2</v>
+        <f>$B$111+($I$2*D120)</f>
+        <v>0.12479999999999999</v>
       </c>
       <c r="G120" s="5">
-        <f t="shared" si="56"/>
-        <v>0.01</v>
+        <f t="shared" si="53"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H120" s="5">
         <f t="shared" si="45"/>
-        <v>4.9806023732074815E-2</v>
+        <v>9.231028741303228E-2</v>
       </c>
       <c r="I120">
+        <f t="shared" si="48"/>
+        <v>1.4774713723470398</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="46"/>
+        <v>4.6512367549477324E-3</v>
+      </c>
+      <c r="K120">
+        <f>J120/$C$111</f>
+        <v>7.7520612582462206E-4</v>
+      </c>
+      <c r="L120">
+        <f t="shared" si="49"/>
+        <v>1905.9077619844479</v>
+      </c>
+      <c r="M120">
+        <f t="shared" si="50"/>
+        <v>5.294188227734578</v>
+      </c>
+      <c r="N120">
         <f t="shared" si="51"/>
-        <v>0.82639121985906172</v>
-      </c>
-      <c r="J120">
-        <f t="shared" si="48"/>
-        <v>3.4728822456614461E-3</v>
+        <v>317.65129366407467</v>
       </c>
       <c r="Q120" s="11"/>
       <c r="R120" s="8"/>
@@ -18925,38 +18956,54 @@
     </row>
     <row r="121" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>71</v>
-      </c>
-      <c r="C121">
-        <f>C120/360</f>
-        <v>141.52476325246346</v>
+        <v>74</v>
+      </c>
+      <c r="C121" s="13">
+        <f>(C118 *C120)/SQRT(POWER(C114,2)+POWER(C118,2))</f>
+        <v>2.7993163294027559</v>
       </c>
       <c r="D121">
         <v>13</v>
       </c>
       <c r="E121">
-        <f t="shared" si="46"/>
-        <v>79.367909729909982</v>
+        <f t="shared" si="47"/>
+        <v>49.070763901605154</v>
       </c>
       <c r="F121" s="5">
-        <f t="shared" si="47"/>
-        <v>5.4199999999999998E-2</v>
+        <f>$B$111+($I$2*D121)</f>
+        <v>0.12820000000000001</v>
       </c>
       <c r="G121" s="5">
-        <f t="shared" si="56"/>
-        <v>0.01</v>
+        <f t="shared" si="53"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H121" s="5">
         <f t="shared" si="45"/>
-        <v>5.3269503470559962E-2</v>
+        <v>9.6857571527870931E-2</v>
       </c>
       <c r="I121">
+        <f t="shared" si="48"/>
+        <v>1.3678122847748</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="46"/>
+        <v>4.5472841148386511E-3</v>
+      </c>
+      <c r="K121">
+        <f>J121/$C$111</f>
+        <v>7.5788068580644186E-4</v>
+      </c>
+      <c r="L121">
+        <f t="shared" si="49"/>
+        <v>1804.7857801249352</v>
+      </c>
+      <c r="M121">
+        <f t="shared" si="50"/>
+        <v>5.0132938336803754</v>
+      </c>
+      <c r="N121">
         <f t="shared" si="51"/>
-        <v>0.72074848624887977</v>
-      </c>
-      <c r="J121">
-        <f t="shared" si="48"/>
-        <v>3.4634797384851465E-3</v>
+        <v>300.79763002082251</v>
       </c>
       <c r="Q121" s="11"/>
       <c r="R121" s="8"/>
@@ -18971,39 +19018,48 @@
       <c r="AA121" s="8"/>
     </row>
     <row r="122" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
-        <v>72</v>
-      </c>
-      <c r="C122">
-        <f>C121*60</f>
-        <v>8491.4857951478079</v>
-      </c>
       <c r="D122">
         <v>14</v>
       </c>
       <c r="E122">
-        <f t="shared" si="46"/>
-        <v>80.002156512432251</v>
+        <f t="shared" si="47"/>
+        <v>50.342222534012144</v>
       </c>
       <c r="F122" s="5">
-        <f t="shared" si="47"/>
-        <v>5.7599999999999998E-2</v>
+        <f>$B$111+($I$2*D122)</f>
+        <v>0.13159999999999999</v>
       </c>
       <c r="G122" s="5">
-        <f t="shared" si="56"/>
-        <v>0.01</v>
+        <f t="shared" si="53"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H122" s="5">
         <f t="shared" si="45"/>
-        <v>5.6725302996105717E-2</v>
+        <v>0.10131490098833747</v>
       </c>
       <c r="I122">
+        <f t="shared" si="48"/>
+        <v>1.2714586324069899</v>
+      </c>
+      <c r="J122">
+        <f t="shared" si="46"/>
+        <v>4.4573294604665359E-3</v>
+      </c>
+      <c r="K122">
+        <f>J122/$C$111</f>
+        <v>7.4288824341108928E-4</v>
+      </c>
+      <c r="L122">
+        <f t="shared" si="49"/>
+        <v>1711.5072740536123</v>
+      </c>
+      <c r="M122">
+        <f t="shared" si="50"/>
+        <v>4.7541868723711449</v>
+      </c>
+      <c r="N122">
         <f t="shared" si="51"/>
-        <v>0.6342467825222684</v>
-      </c>
-      <c r="J122">
-        <f t="shared" si="48"/>
-        <v>3.4557995255457552E-3</v>
+        <v>285.25121234226867</v>
       </c>
       <c r="Q122" s="8"/>
       <c r="R122" s="8"/>
@@ -19018,32 +19074,55 @@
       <c r="AA122" s="8"/>
     </row>
     <row r="123" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>77</v>
+      </c>
+      <c r="C123">
+        <f>SQRT(POWER(C114,2)+POWER(C118,2))</f>
+        <v>4525.5053058519188</v>
+      </c>
       <c r="D123">
         <v>15</v>
       </c>
       <c r="E123">
-        <f t="shared" si="46"/>
-        <v>80.56466127669681</v>
+        <f t="shared" si="47"/>
+        <v>51.52834052354055</v>
       </c>
       <c r="F123" s="5">
-        <f t="shared" si="47"/>
-        <v>6.0999999999999999E-2</v>
+        <f>$B$111+($I$2*D123)</f>
+        <v>0.13500000000000001</v>
       </c>
       <c r="G123" s="5">
-        <f t="shared" si="56"/>
-        <v>0.01</v>
+        <f t="shared" si="53"/>
+        <v>8.3987206393136865E-2</v>
       </c>
       <c r="H123" s="5">
         <f t="shared" si="45"/>
-        <v>6.0174745533321534E-2</v>
+        <v>0.10569365715253037</v>
       </c>
       <c r="I123">
         <f>E123-E122</f>
-        <v>0.56250476426455975</v>
+        <v>1.1861179895284053</v>
       </c>
       <c r="J123">
-        <f t="shared" si="48"/>
-        <v>3.4494425372158175E-3</v>
+        <f t="shared" si="46"/>
+        <v>4.3787561641929068E-3</v>
+      </c>
+      <c r="K123">
+        <f>J123/$C$111</f>
+        <v>7.2979269403215113E-4</v>
+      </c>
+      <c r="L123">
+        <f t="shared" si="49"/>
+        <v>1625.2807122184629</v>
+      </c>
+      <c r="M123">
+        <f t="shared" si="50"/>
+        <v>4.5146686450512856</v>
+      </c>
+      <c r="N123">
+        <f t="shared" si="51"/>
+        <v>270.88011870307713</v>
       </c>
       <c r="Q123" s="8"/>
       <c r="R123" s="8"/>
@@ -19074,155 +19153,101 @@
       <c r="AA124" s="8"/>
     </row>
     <row r="125" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
-        <v>78</v>
-      </c>
-      <c r="C125">
-        <v>500</v>
-      </c>
       <c r="G125" s="5"/>
       <c r="H125" s="5"/>
       <c r="J125" s="5"/>
     </row>
     <row r="126" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
-        <v>76</v>
-      </c>
-      <c r="C126">
-        <v>100</v>
-      </c>
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
       <c r="J126" s="5"/>
     </row>
     <row r="127" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B127" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C127">
-        <f>1/(2*3.1416*C126*C125)</f>
-        <v>3.1830914183855364E-6</v>
-      </c>
       <c r="G127" s="5"/>
       <c r="H127" s="5"/>
       <c r="J127" s="5"/>
     </row>
     <row r="128" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C128" s="4"/>
       <c r="G128" s="5"/>
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
-        <v>74</v>
-      </c>
-      <c r="C129">
-        <f>C121</f>
-        <v>141.52476325246346</v>
-      </c>
+    <row r="129" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G129" s="5"/>
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B130" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C130" s="13">
-        <f>1/(2*3.1416*C129*C127)</f>
-        <v>353.29506194478415</v>
-      </c>
+    <row r="130" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G130" s="5"/>
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G131" s="5"/>
       <c r="H131" s="5"/>
       <c r="I131" s="5"/>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B132" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C132">
-        <v>2.8</v>
-      </c>
+    <row r="132" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G132" s="5"/>
       <c r="H132" s="5"/>
       <c r="I132" s="5"/>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
-        <v>77</v>
-      </c>
-      <c r="C133" s="13">
-        <f>(C130 *C132)/SQRT(POWER(C126,2)+POWER(C130,2))</f>
-        <v>2.6941552837864267</v>
-      </c>
+    <row r="133" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G133" s="5"/>
       <c r="H133" s="5"/>
       <c r="I133" s="5"/>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G134" s="5"/>
       <c r="H134" s="5"/>
       <c r="I134" s="5"/>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
-        <v>80</v>
-      </c>
-      <c r="C135">
-        <f>SQRT(POWER(C126,2)+POWER(C130,2))</f>
-        <v>367.17489129101529</v>
-      </c>
+    <row r="135" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G135" s="5"/>
       <c r="H135" s="5"/>
       <c r="I135" s="5"/>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G136" s="5"/>
       <c r="H136" s="5"/>
       <c r="I136" s="5"/>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G137" s="5"/>
       <c r="H137" s="5"/>
       <c r="I137" s="5"/>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G138" s="5"/>
       <c r="H138" s="5"/>
       <c r="I138" s="5"/>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G139" s="5"/>
       <c r="H139" s="5"/>
       <c r="I139" s="5"/>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G140" s="5"/>
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G141" s="5"/>
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G142" s="5"/>
       <c r="H142" s="5"/>
       <c r="I142" s="5"/>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G143" s="5"/>
       <c r="H143" s="5"/>
       <c r="I143" s="5"/>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G144" s="5"/>
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
@@ -19243,8 +19268,7 @@
       <c r="I147" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B108:C108"/>
+  <mergeCells count="4">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="D4:F4"/>
@@ -19260,7 +19284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3BDFF7-A03C-4436-BDC7-9DE4C8404CC4}">
   <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -19284,7 +19308,7 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -19345,7 +19369,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H8" s="18">
         <v>14</v>
@@ -19356,7 +19380,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H9">
         <f>SUM(H4:H8)</f>
@@ -19374,7 +19398,7 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H11">
         <f>L5/H9</f>
@@ -19387,7 +19411,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H12">
         <f>H11/4</f>
@@ -19400,7 +19424,7 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C14">
         <v>92.5</v>
@@ -19408,7 +19432,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C15">
         <v>50000000</v>
@@ -19416,7 +19440,7 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16">
         <v>4.9999999999999997E-12</v>
@@ -19428,7 +19452,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -19436,7 +19460,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C18">
         <v>3900</v>
@@ -19444,13 +19468,13 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -19473,7 +19497,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -19526,13 +19550,13 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="6:11" x14ac:dyDescent="0.25">
@@ -19554,7 +19578,7 @@
         <v>3.7138888888888889E-5</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="6:11" x14ac:dyDescent="0.25">
@@ -19573,7 +19597,7 @@
         <v>1.0277777777777777E-5</v>
       </c>
       <c r="K8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="6:11" x14ac:dyDescent="0.25">
@@ -19592,7 +19616,7 @@
         <v>7.6916666666666662E-5</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="6:11" x14ac:dyDescent="0.25">
@@ -19611,7 +19635,7 @@
         <v>1.548611111111111E-5</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="6:11" x14ac:dyDescent="0.25">
@@ -19630,7 +19654,7 @@
         <v>6.0854166666666663E-4</v>
       </c>
       <c r="K11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="6:11" x14ac:dyDescent="0.25">
@@ -19649,7 +19673,7 @@
         <v>2.1638888888888888E-5</v>
       </c>
       <c r="K12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="6:11" x14ac:dyDescent="0.25">
@@ -19668,7 +19692,7 @@
         <v>3.8597222222222222E-5</v>
       </c>
       <c r="K13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="6:11" x14ac:dyDescent="0.25">
@@ -19687,7 +19711,7 @@
         <v>9.4569444444444445E-5</v>
       </c>
       <c r="K14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="6:11" x14ac:dyDescent="0.25">
@@ -19706,7 +19730,7 @@
         <v>4.6458333333333335E-5</v>
       </c>
       <c r="K15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="6:11" x14ac:dyDescent="0.25">
@@ -19796,37 +19820,37 @@
   <sheetData>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" t="s">
         <v>81</v>
       </c>
-      <c r="C4" t="s">
+      <c r="O4" t="s">
         <v>82</v>
       </c>
-      <c r="F4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="P4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q4" t="s">
         <v>86</v>
-      </c>
-      <c r="L4" t="s">
-        <v>83</v>
-      </c>
-      <c r="M4" t="s">
-        <v>84</v>
-      </c>
-      <c r="O4" t="s">
-        <v>85</v>
-      </c>
-      <c r="P4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Non plus ultra changes
</commit_message>
<xml_diff>
--- a/Encoder Characteristics.xlsx
+++ b/Encoder Characteristics.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pauld\Programming\NN54\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D9AFD1-C1BF-4F91-BAAD-4C393F14F229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A98068E-0C82-4EF8-B08D-482B7921E9C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encoder Error" sheetId="1" r:id="rId1"/>
     <sheet name="Angle" sheetId="2" r:id="rId2"/>
     <sheet name="Battery Consumption" sheetId="3" r:id="rId3"/>
     <sheet name="Cycle Counting" sheetId="4" r:id="rId4"/>
-    <sheet name="ADC" sheetId="5" r:id="rId5"/>
+    <sheet name="Antenna" sheetId="6" r:id="rId5"/>
+    <sheet name="ADC" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="94">
   <si>
     <t>Number of measurments</t>
   </si>
@@ -301,6 +302,21 @@
   </si>
   <si>
     <t>init length</t>
+  </si>
+  <si>
+    <t>Critical Length</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Eff</t>
+  </si>
+  <si>
+    <t>Mhz</t>
   </si>
 </sst>
 </file>
@@ -19519,7 +19535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1AC376-52B3-4B27-BBC6-391D349B9994}">
   <dimension ref="F4:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="168" workbookViewId="0">
+    <sheetView topLeftCell="D4" zoomScale="168" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -19803,6 +19819,64 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA989DE8-DF33-4045-B12C-91983CAB0821}">
+  <dimension ref="C10:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4">
+        <v>300000000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11">
+        <v>2448</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="4">
+        <f>(D10/D11)*(1/SQRT(D12))*(1/12)</f>
+        <v>5538.4614434910163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9794E4-8E8D-461D-9918-F078072C3809}">
   <dimension ref="A4:Q58"/>
   <sheetViews>

</xml_diff>